<commit_message>
Hyperlinks restored and Deduped with PDFs
</commit_message>
<xml_diff>
--- a/book/DATA/phase1_document_registry_MASTER_hyperlinks_restored.xlsx
+++ b/book/DATA/phase1_document_registry_MASTER_hyperlinks_restored.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\aimoralcode-core\book\DATA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F1D0A4-F1BA-492E-8C4D-E427F2CEE29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -6147,8 +6153,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6224,13 +6230,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6268,7 +6282,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -6302,6 +6316,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -6336,9 +6351,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6511,14 +6527,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q294"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="19.44140625" customWidth="1"/>
+    <col min="12" max="12" width="24.77734375" customWidth="1"/>
+    <col min="13" max="13" width="23.6640625" customWidth="1"/>
+    <col min="14" max="14" width="30.88671875" customWidth="1"/>
+    <col min="15" max="15" width="28.6640625" customWidth="1"/>
+    <col min="16" max="16" width="24.5546875" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6571,7 +6599,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -6612,7 +6640,7 @@
         <v>1779</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -6656,7 +6684,7 @@
         <v>1780</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -6700,7 +6728,7 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -6744,7 +6772,7 @@
         <v>1782</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -6788,7 +6816,7 @@
         <v>1783</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -6832,7 +6860,7 @@
         <v>1784</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -6876,7 +6904,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -6920,7 +6948,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -6964,7 +6992,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -7008,7 +7036,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -7052,7 +7080,7 @@
         <v>1789</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -7096,7 +7124,7 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -7140,7 +7168,7 @@
         <v>1791</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -7184,7 +7212,7 @@
         <v>1792</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -7228,7 +7256,7 @@
         <v>1785</v>
       </c>
     </row>
-    <row r="17" spans="1:15">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -7272,7 +7300,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -7316,7 +7344,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -7360,7 +7388,7 @@
         <v>1793</v>
       </c>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -7404,7 +7432,7 @@
         <v>1794</v>
       </c>
     </row>
-    <row r="21" spans="1:15">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -7448,7 +7476,7 @@
         <v>1795</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>37</v>
       </c>
@@ -7492,7 +7520,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -7536,7 +7564,7 @@
         <v>1797</v>
       </c>
     </row>
-    <row r="24" spans="1:15">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -7577,7 +7605,7 @@
         <v>1538</v>
       </c>
     </row>
-    <row r="25" spans="1:15">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -7615,7 +7643,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="26" spans="1:15">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -7656,7 +7684,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -7700,7 +7728,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="28" spans="1:15">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -7744,7 +7772,7 @@
         <v>1799</v>
       </c>
     </row>
-    <row r="29" spans="1:15">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -7788,7 +7816,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="30" spans="1:15">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -7829,7 +7857,7 @@
         <v>1543</v>
       </c>
     </row>
-    <row r="31" spans="1:15">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -7870,7 +7898,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="32" spans="1:15">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -7914,7 +7942,7 @@
         <v>1801</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -7958,7 +7986,7 @@
         <v>1802</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -8002,7 +8030,7 @@
         <v>1788</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -8043,7 +8071,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -8084,7 +8112,7 @@
         <v>1803</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -8128,7 +8156,7 @@
         <v>1804</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -8172,7 +8200,7 @@
         <v>1805</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -8216,7 +8244,7 @@
         <v>1806</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -8260,7 +8288,7 @@
         <v>1807</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -8301,7 +8329,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -8339,7 +8367,7 @@
         <v>1553</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>58</v>
       </c>
@@ -8380,7 +8408,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>59</v>
       </c>
@@ -8424,7 +8452,7 @@
         <v>1810</v>
       </c>
     </row>
-    <row r="45" spans="1:15">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -8468,7 +8496,7 @@
         <v>1811</v>
       </c>
     </row>
-    <row r="46" spans="1:15">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>61</v>
       </c>
@@ -8509,7 +8537,7 @@
         <v>1557</v>
       </c>
     </row>
-    <row r="47" spans="1:15">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -8553,7 +8581,7 @@
         <v>1812</v>
       </c>
     </row>
-    <row r="48" spans="1:15">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>63</v>
       </c>
@@ -8597,7 +8625,7 @@
         <v>1813</v>
       </c>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>64</v>
       </c>
@@ -8641,7 +8669,7 @@
         <v>1814</v>
       </c>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>65</v>
       </c>
@@ -8685,7 +8713,7 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -8729,7 +8757,7 @@
         <v>1816</v>
       </c>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>67</v>
       </c>
@@ -8773,7 +8801,7 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -8814,7 +8842,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -8858,7 +8886,7 @@
         <v>1819</v>
       </c>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -8902,7 +8930,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="56" spans="1:15">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -8943,7 +8971,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -8984,7 +9012,7 @@
         <v>1796</v>
       </c>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -9028,7 +9056,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -9072,7 +9100,7 @@
         <v>1822</v>
       </c>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -9113,7 +9141,7 @@
         <v>1823</v>
       </c>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -9157,7 +9185,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -9201,7 +9229,7 @@
         <v>1825</v>
       </c>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -9245,7 +9273,7 @@
         <v>1826</v>
       </c>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -9289,7 +9317,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="65" spans="1:15">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -9333,7 +9361,7 @@
         <v>1828</v>
       </c>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -9374,7 +9402,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -9415,7 +9443,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -9459,7 +9487,7 @@
         <v>1830</v>
       </c>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -9503,7 +9531,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -9544,7 +9572,7 @@
         <v>1580</v>
       </c>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -9585,7 +9613,7 @@
         <v>1832</v>
       </c>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -9629,7 +9657,7 @@
         <v>1833</v>
       </c>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>88</v>
       </c>
@@ -9673,7 +9701,7 @@
         <v>1834</v>
       </c>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>89</v>
       </c>
@@ -9714,7 +9742,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -9755,7 +9783,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>91</v>
       </c>
@@ -9793,7 +9821,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>92</v>
       </c>
@@ -9834,7 +9862,7 @@
         <v>1836</v>
       </c>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>93</v>
       </c>
@@ -9875,7 +9903,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>94</v>
       </c>
@@ -9916,7 +9944,7 @@
         <v>1837</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>95</v>
       </c>
@@ -9957,7 +9985,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="81" spans="1:15">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>96</v>
       </c>
@@ -9998,7 +10026,7 @@
         <v>1838</v>
       </c>
     </row>
-    <row r="82" spans="1:15">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>97</v>
       </c>
@@ -10042,7 +10070,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="83" spans="1:15">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>98</v>
       </c>
@@ -10086,7 +10114,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="84" spans="1:15">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>99</v>
       </c>
@@ -10127,7 +10155,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="85" spans="1:15">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>100</v>
       </c>
@@ -10165,7 +10193,7 @@
         <v>1595</v>
       </c>
     </row>
-    <row r="86" spans="1:15">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>101</v>
       </c>
@@ -10206,7 +10234,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="87" spans="1:15">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>102</v>
       </c>
@@ -10247,7 +10275,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="88" spans="1:15">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -10291,7 +10319,7 @@
         <v>1843</v>
       </c>
     </row>
-    <row r="89" spans="1:15">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>104</v>
       </c>
@@ -10335,7 +10363,7 @@
         <v>1844</v>
       </c>
     </row>
-    <row r="90" spans="1:15">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>105</v>
       </c>
@@ -10376,7 +10404,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="91" spans="1:15">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>106</v>
       </c>
@@ -10420,7 +10448,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="92" spans="1:15">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -10458,7 +10486,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="93" spans="1:15">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -10502,7 +10530,7 @@
         <v>1847</v>
       </c>
     </row>
-    <row r="94" spans="1:15">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>109</v>
       </c>
@@ -10543,7 +10571,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>110</v>
       </c>
@@ -10587,7 +10615,7 @@
         <v>1849</v>
       </c>
     </row>
-    <row r="96" spans="1:15">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>111</v>
       </c>
@@ -10625,7 +10653,7 @@
         <v>1606</v>
       </c>
     </row>
-    <row r="97" spans="1:15">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>112</v>
       </c>
@@ -10663,7 +10691,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="98" spans="1:15">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>113</v>
       </c>
@@ -10704,7 +10732,7 @@
         <v>1850</v>
       </c>
     </row>
-    <row r="99" spans="1:15">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -10745,7 +10773,7 @@
         <v>1851</v>
       </c>
     </row>
-    <row r="100" spans="1:15">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>115</v>
       </c>
@@ -10789,7 +10817,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="101" spans="1:15">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>116</v>
       </c>
@@ -10830,7 +10858,7 @@
         <v>1853</v>
       </c>
     </row>
-    <row r="102" spans="1:15">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>117</v>
       </c>
@@ -10871,7 +10899,7 @@
         <v>1854</v>
       </c>
     </row>
-    <row r="103" spans="1:15">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>118</v>
       </c>
@@ -10915,7 +10943,7 @@
         <v>1855</v>
       </c>
     </row>
-    <row r="104" spans="1:15">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>119</v>
       </c>
@@ -10959,7 +10987,7 @@
         <v>1856</v>
       </c>
     </row>
-    <row r="105" spans="1:15">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>120</v>
       </c>
@@ -11000,7 +11028,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="106" spans="1:15">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>121</v>
       </c>
@@ -11041,7 +11069,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="107" spans="1:15">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>122</v>
       </c>
@@ -11085,7 +11113,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="108" spans="1:15">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -11129,7 +11157,7 @@
         <v>1859</v>
       </c>
     </row>
-    <row r="109" spans="1:15">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>124</v>
       </c>
@@ -11173,7 +11201,7 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="110" spans="1:15">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>125</v>
       </c>
@@ -11217,7 +11245,7 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="111" spans="1:15">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>126</v>
       </c>
@@ -11261,7 +11289,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>127</v>
       </c>
@@ -11302,7 +11330,7 @@
         <v>1827</v>
       </c>
     </row>
-    <row r="113" spans="1:15">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>128</v>
       </c>
@@ -11346,7 +11374,7 @@
         <v>1862</v>
       </c>
     </row>
-    <row r="114" spans="1:15">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>129</v>
       </c>
@@ -11390,7 +11418,7 @@
         <v>1863</v>
       </c>
     </row>
-    <row r="115" spans="1:15">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>130</v>
       </c>
@@ -11434,7 +11462,7 @@
         <v>1864</v>
       </c>
     </row>
-    <row r="116" spans="1:15">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>131</v>
       </c>
@@ -11478,7 +11506,7 @@
         <v>1865</v>
       </c>
     </row>
-    <row r="117" spans="1:15">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>132</v>
       </c>
@@ -11522,7 +11550,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="118" spans="1:15">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>133</v>
       </c>
@@ -11566,7 +11594,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="119" spans="1:15">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>134</v>
       </c>
@@ -11610,7 +11638,7 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="120" spans="1:15">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>135</v>
       </c>
@@ -11654,7 +11682,7 @@
         <v>1869</v>
       </c>
     </row>
-    <row r="121" spans="1:15">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>136</v>
       </c>
@@ -11698,7 +11726,7 @@
         <v>1870</v>
       </c>
     </row>
-    <row r="122" spans="1:15">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>137</v>
       </c>
@@ -11742,7 +11770,7 @@
         <v>1871</v>
       </c>
     </row>
-    <row r="123" spans="1:15">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>138</v>
       </c>
@@ -11786,7 +11814,7 @@
         <v>1872</v>
       </c>
     </row>
-    <row r="124" spans="1:15">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>139</v>
       </c>
@@ -11830,7 +11858,7 @@
         <v>1873</v>
       </c>
     </row>
-    <row r="125" spans="1:15">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>140</v>
       </c>
@@ -11874,7 +11902,7 @@
         <v>1874</v>
       </c>
     </row>
-    <row r="126" spans="1:15">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>141</v>
       </c>
@@ -11918,7 +11946,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="127" spans="1:15">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>142</v>
       </c>
@@ -11962,7 +11990,7 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="128" spans="1:15">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>143</v>
       </c>
@@ -12003,7 +12031,7 @@
         <v>1877</v>
       </c>
     </row>
-    <row r="129" spans="1:15">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -12047,7 +12075,7 @@
         <v>1878</v>
       </c>
     </row>
-    <row r="130" spans="1:15">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>145</v>
       </c>
@@ -12091,7 +12119,7 @@
         <v>1879</v>
       </c>
     </row>
-    <row r="131" spans="1:15">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>146</v>
       </c>
@@ -12135,7 +12163,7 @@
         <v>1880</v>
       </c>
     </row>
-    <row r="132" spans="1:15">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -12179,7 +12207,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="133" spans="1:15">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>148</v>
       </c>
@@ -12220,7 +12248,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="134" spans="1:15">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>149</v>
       </c>
@@ -12261,7 +12289,7 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="135" spans="1:15">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>150</v>
       </c>
@@ -12305,7 +12333,7 @@
         <v>1883</v>
       </c>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -12349,7 +12377,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>152</v>
       </c>
@@ -12390,7 +12418,7 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>153</v>
       </c>
@@ -12434,7 +12462,7 @@
         <v>1886</v>
       </c>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>154</v>
       </c>
@@ -12478,7 +12506,7 @@
         <v>1887</v>
       </c>
     </row>
-    <row r="140" spans="1:15">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>155</v>
       </c>
@@ -12519,7 +12547,7 @@
         <v>1888</v>
       </c>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>156</v>
       </c>
@@ -12560,7 +12588,7 @@
         <v>1889</v>
       </c>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>157</v>
       </c>
@@ -12604,7 +12632,7 @@
         <v>1890</v>
       </c>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>158</v>
       </c>
@@ -12648,7 +12676,7 @@
         <v>1891</v>
       </c>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>159</v>
       </c>
@@ -12689,7 +12717,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="145" spans="1:15">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>160</v>
       </c>
@@ -12730,7 +12758,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="146" spans="1:15">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>161</v>
       </c>
@@ -12774,7 +12802,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="147" spans="1:15">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>162</v>
       </c>
@@ -12818,7 +12846,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="148" spans="1:15">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>163</v>
       </c>
@@ -12862,7 +12890,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="149" spans="1:15">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>164</v>
       </c>
@@ -12903,7 +12931,7 @@
         <v>1894</v>
       </c>
     </row>
-    <row r="150" spans="1:15">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>165</v>
       </c>
@@ -12947,7 +12975,7 @@
         <v>1895</v>
       </c>
     </row>
-    <row r="151" spans="1:15">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>166</v>
       </c>
@@ -12991,7 +13019,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="152" spans="1:15">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>167</v>
       </c>
@@ -13032,7 +13060,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="153" spans="1:15">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>168</v>
       </c>
@@ -13076,7 +13104,7 @@
         <v>1816</v>
       </c>
     </row>
-    <row r="154" spans="1:15">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>169</v>
       </c>
@@ -13120,7 +13148,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="155" spans="1:15">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>170</v>
       </c>
@@ -13164,7 +13192,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="156" spans="1:15">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>171</v>
       </c>
@@ -13208,7 +13236,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>172</v>
       </c>
@@ -13246,7 +13274,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="158" spans="1:15">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>173</v>
       </c>
@@ -13287,7 +13315,7 @@
         <v>1901</v>
       </c>
     </row>
-    <row r="159" spans="1:15">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>174</v>
       </c>
@@ -13325,7 +13353,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="160" spans="1:15">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>175</v>
       </c>
@@ -13366,7 +13394,7 @@
         <v>1902</v>
       </c>
     </row>
-    <row r="161" spans="1:15">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>176</v>
       </c>
@@ -13410,7 +13438,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="162" spans="1:15">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>177</v>
       </c>
@@ -13451,7 +13479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:15">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>178</v>
       </c>
@@ -13492,7 +13520,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="164" spans="1:15">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>179</v>
       </c>
@@ -13536,7 +13564,7 @@
         <v>1904</v>
       </c>
     </row>
-    <row r="165" spans="1:15">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>180</v>
       </c>
@@ -13580,7 +13608,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="166" spans="1:15">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>181</v>
       </c>
@@ -13624,7 +13652,7 @@
         <v>1906</v>
       </c>
     </row>
-    <row r="167" spans="1:15">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>182</v>
       </c>
@@ -13665,7 +13693,7 @@
         <v>1907</v>
       </c>
     </row>
-    <row r="168" spans="1:15">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>183</v>
       </c>
@@ -13703,7 +13731,7 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="169" spans="1:15">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>184</v>
       </c>
@@ -13747,7 +13775,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="170" spans="1:15">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>185</v>
       </c>
@@ -13791,7 +13819,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="171" spans="1:15">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>186</v>
       </c>
@@ -13835,7 +13863,7 @@
         <v>1909</v>
       </c>
     </row>
-    <row r="172" spans="1:15">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>187</v>
       </c>
@@ -13879,7 +13907,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="173" spans="1:15">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>188</v>
       </c>
@@ -13920,7 +13948,7 @@
         <v>1911</v>
       </c>
     </row>
-    <row r="174" spans="1:15">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>189</v>
       </c>
@@ -13964,7 +13992,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="175" spans="1:15">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>190</v>
       </c>
@@ -14005,7 +14033,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="176" spans="1:15">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>191</v>
       </c>
@@ -14049,7 +14077,7 @@
         <v>1914</v>
       </c>
     </row>
-    <row r="177" spans="1:15">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>192</v>
       </c>
@@ -14093,7 +14121,7 @@
         <v>1915</v>
       </c>
     </row>
-    <row r="178" spans="1:15">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>193</v>
       </c>
@@ -14137,7 +14165,7 @@
         <v>1916</v>
       </c>
     </row>
-    <row r="179" spans="1:15">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>194</v>
       </c>
@@ -14181,7 +14209,7 @@
         <v>1917</v>
       </c>
     </row>
-    <row r="180" spans="1:15">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>195</v>
       </c>
@@ -14225,7 +14253,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="181" spans="1:15">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>196</v>
       </c>
@@ -14269,7 +14297,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="182" spans="1:15">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>197</v>
       </c>
@@ -14313,7 +14341,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="183" spans="1:15">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>198</v>
       </c>
@@ -14357,7 +14385,7 @@
         <v>1918</v>
       </c>
     </row>
-    <row r="184" spans="1:15">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>199</v>
       </c>
@@ -14401,7 +14429,7 @@
         <v>1921</v>
       </c>
     </row>
-    <row r="185" spans="1:15">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>200</v>
       </c>
@@ -14445,7 +14473,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="186" spans="1:15">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>201</v>
       </c>
@@ -14489,7 +14517,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="187" spans="1:15">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>202</v>
       </c>
@@ -14533,7 +14561,7 @@
         <v>1858</v>
       </c>
     </row>
-    <row r="188" spans="1:15">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>203</v>
       </c>
@@ -14577,7 +14605,7 @@
         <v>1899</v>
       </c>
     </row>
-    <row r="189" spans="1:15">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>204</v>
       </c>
@@ -14621,7 +14649,7 @@
         <v>1922</v>
       </c>
     </row>
-    <row r="190" spans="1:15">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>205</v>
       </c>
@@ -14662,7 +14690,7 @@
         <v>1923</v>
       </c>
     </row>
-    <row r="191" spans="1:15">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>206</v>
       </c>
@@ -14706,7 +14734,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="192" spans="1:15">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>207</v>
       </c>
@@ -14750,7 +14778,7 @@
         <v>1925</v>
       </c>
     </row>
-    <row r="193" spans="1:15">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>208</v>
       </c>
@@ -14791,7 +14819,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="194" spans="1:15">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>209</v>
       </c>
@@ -14835,7 +14863,7 @@
         <v>1821</v>
       </c>
     </row>
-    <row r="195" spans="1:15">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>210</v>
       </c>
@@ -14879,7 +14907,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="196" spans="1:15">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>211</v>
       </c>
@@ -14923,7 +14951,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="197" spans="1:15">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>212</v>
       </c>
@@ -14964,7 +14992,7 @@
         <v>1926</v>
       </c>
     </row>
-    <row r="198" spans="1:15">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>213</v>
       </c>
@@ -15008,7 +15036,7 @@
         <v>1927</v>
       </c>
     </row>
-    <row r="199" spans="1:15">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>214</v>
       </c>
@@ -15052,7 +15080,7 @@
         <v>1928</v>
       </c>
     </row>
-    <row r="200" spans="1:15">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>215</v>
       </c>
@@ -15096,7 +15124,7 @@
         <v>1929</v>
       </c>
     </row>
-    <row r="201" spans="1:15">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>216</v>
       </c>
@@ -15137,7 +15165,7 @@
         <v>1930</v>
       </c>
     </row>
-    <row r="202" spans="1:15">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>217</v>
       </c>
@@ -15178,7 +15206,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="203" spans="1:15">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>218</v>
       </c>
@@ -15222,7 +15250,7 @@
         <v>1931</v>
       </c>
     </row>
-    <row r="204" spans="1:15">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>219</v>
       </c>
@@ -15263,7 +15291,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="205" spans="1:15">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>220</v>
       </c>
@@ -15307,7 +15335,7 @@
         <v>1933</v>
       </c>
     </row>
-    <row r="206" spans="1:15">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>221</v>
       </c>
@@ -15351,7 +15379,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="207" spans="1:15">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>222</v>
       </c>
@@ -15392,7 +15420,7 @@
         <v>1935</v>
       </c>
     </row>
-    <row r="208" spans="1:15">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>223</v>
       </c>
@@ -15436,7 +15464,7 @@
         <v>1936</v>
       </c>
     </row>
-    <row r="209" spans="1:15">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>224</v>
       </c>
@@ -15480,7 +15508,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="210" spans="1:15">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>225</v>
       </c>
@@ -15521,7 +15549,7 @@
         <v>1938</v>
       </c>
     </row>
-    <row r="211" spans="1:15">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>226</v>
       </c>
@@ -15562,7 +15590,7 @@
         <v>1939</v>
       </c>
     </row>
-    <row r="212" spans="1:15">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>227</v>
       </c>
@@ -15606,7 +15634,7 @@
         <v>1940</v>
       </c>
     </row>
-    <row r="213" spans="1:15">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>228</v>
       </c>
@@ -15650,7 +15678,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="214" spans="1:15">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>229</v>
       </c>
@@ -15694,7 +15722,7 @@
         <v>1941</v>
       </c>
     </row>
-    <row r="215" spans="1:15">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>230</v>
       </c>
@@ -15738,7 +15766,7 @@
         <v>1942</v>
       </c>
     </row>
-    <row r="216" spans="1:15">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>231</v>
       </c>
@@ -15782,7 +15810,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="217" spans="1:15">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>232</v>
       </c>
@@ -15823,7 +15851,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="218" spans="1:15">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>233</v>
       </c>
@@ -15867,7 +15895,7 @@
         <v>1944</v>
       </c>
     </row>
-    <row r="219" spans="1:15">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>234</v>
       </c>
@@ -15908,7 +15936,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="220" spans="1:15">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>235</v>
       </c>
@@ -15949,7 +15977,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="221" spans="1:15">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>236</v>
       </c>
@@ -15987,7 +16015,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="222" spans="1:15">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>237</v>
       </c>
@@ -16031,7 +16059,7 @@
         <v>1946</v>
       </c>
     </row>
-    <row r="223" spans="1:15">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>238</v>
       </c>
@@ -16072,7 +16100,7 @@
         <v>1947</v>
       </c>
     </row>
-    <row r="224" spans="1:15">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>239</v>
       </c>
@@ -16116,7 +16144,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="225" spans="1:15">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>240</v>
       </c>
@@ -16160,7 +16188,7 @@
         <v>1949</v>
       </c>
     </row>
-    <row r="226" spans="1:15">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>241</v>
       </c>
@@ -16201,7 +16229,7 @@
         <v>1950</v>
       </c>
     </row>
-    <row r="227" spans="1:15">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>242</v>
       </c>
@@ -16245,7 +16273,7 @@
         <v>1951</v>
       </c>
     </row>
-    <row r="228" spans="1:15">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>243</v>
       </c>
@@ -16289,7 +16317,7 @@
         <v>1905</v>
       </c>
     </row>
-    <row r="229" spans="1:15">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>244</v>
       </c>
@@ -16330,7 +16358,7 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="230" spans="1:15">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>245</v>
       </c>
@@ -16371,7 +16399,7 @@
         <v>1953</v>
       </c>
     </row>
-    <row r="231" spans="1:15">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>246</v>
       </c>
@@ -16412,7 +16440,7 @@
         <v>1816</v>
       </c>
     </row>
-    <row r="232" spans="1:15">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>247</v>
       </c>
@@ -16453,7 +16481,7 @@
         <v>1954</v>
       </c>
     </row>
-    <row r="233" spans="1:15">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>248</v>
       </c>
@@ -16491,7 +16519,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="234" spans="1:15">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>249</v>
       </c>
@@ -16532,7 +16560,7 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="235" spans="1:15">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>250</v>
       </c>
@@ -16573,7 +16601,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="236" spans="1:15">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>251</v>
       </c>
@@ -16614,7 +16642,7 @@
         <v>1957</v>
       </c>
     </row>
-    <row r="237" spans="1:15">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>252</v>
       </c>
@@ -16652,7 +16680,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="238" spans="1:15">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>253</v>
       </c>
@@ -16693,7 +16721,7 @@
         <v>1958</v>
       </c>
     </row>
-    <row r="239" spans="1:15">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>254</v>
       </c>
@@ -16734,7 +16762,7 @@
         <v>1842</v>
       </c>
     </row>
-    <row r="240" spans="1:15">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>255</v>
       </c>
@@ -16778,7 +16806,7 @@
         <v>1959</v>
       </c>
     </row>
-    <row r="241" spans="1:15">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>256</v>
       </c>
@@ -16816,7 +16844,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="242" spans="1:15">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>257</v>
       </c>
@@ -16857,7 +16885,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="243" spans="1:15">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>258</v>
       </c>
@@ -16895,7 +16923,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="244" spans="1:15">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>259</v>
       </c>
@@ -16936,7 +16964,7 @@
         <v>1960</v>
       </c>
     </row>
-    <row r="245" spans="1:15">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>260</v>
       </c>
@@ -16980,7 +17008,7 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="246" spans="1:15">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>261</v>
       </c>
@@ -17024,7 +17052,7 @@
         <v>1962</v>
       </c>
     </row>
-    <row r="247" spans="1:15">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>262</v>
       </c>
@@ -17065,7 +17093,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="248" spans="1:15">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>263</v>
       </c>
@@ -17109,7 +17137,7 @@
         <v>1964</v>
       </c>
     </row>
-    <row r="249" spans="1:15">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>264</v>
       </c>
@@ -17150,7 +17178,7 @@
         <v>1965</v>
       </c>
     </row>
-    <row r="250" spans="1:15">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>265</v>
       </c>
@@ -17191,7 +17219,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="251" spans="1:15">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>266</v>
       </c>
@@ -17232,7 +17260,7 @@
         <v>1852</v>
       </c>
     </row>
-    <row r="252" spans="1:15">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>267</v>
       </c>
@@ -17276,7 +17304,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="253" spans="1:15">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>268</v>
       </c>
@@ -17320,7 +17348,7 @@
         <v>1968</v>
       </c>
     </row>
-    <row r="254" spans="1:15">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>269</v>
       </c>
@@ -17364,7 +17392,7 @@
         <v>1820</v>
       </c>
     </row>
-    <row r="255" spans="1:15">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>270</v>
       </c>
@@ -17408,7 +17436,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="256" spans="1:15">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>271</v>
       </c>
@@ -17452,7 +17480,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="257" spans="1:15">
+    <row r="257" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>272</v>
       </c>
@@ -17496,7 +17524,7 @@
         <v>1971</v>
       </c>
     </row>
-    <row r="258" spans="1:15">
+    <row r="258" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>273</v>
       </c>
@@ -17537,7 +17565,7 @@
         <v>1972</v>
       </c>
     </row>
-    <row r="259" spans="1:15">
+    <row r="259" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>274</v>
       </c>
@@ -17578,7 +17606,7 @@
         <v>1973</v>
       </c>
     </row>
-    <row r="260" spans="1:15">
+    <row r="260" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>275</v>
       </c>
@@ -17622,7 +17650,7 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="261" spans="1:15">
+    <row r="261" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>276</v>
       </c>
@@ -17666,7 +17694,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="262" spans="1:15">
+    <row r="262" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>277</v>
       </c>
@@ -17710,7 +17738,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="263" spans="1:15">
+    <row r="263" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>278</v>
       </c>
@@ -17754,7 +17782,7 @@
         <v>1977</v>
       </c>
     </row>
-    <row r="264" spans="1:15">
+    <row r="264" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>279</v>
       </c>
@@ -17798,7 +17826,7 @@
         <v>1978</v>
       </c>
     </row>
-    <row r="265" spans="1:15">
+    <row r="265" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>280</v>
       </c>
@@ -17839,7 +17867,7 @@
         <v>1979</v>
       </c>
     </row>
-    <row r="266" spans="1:15">
+    <row r="266" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>281</v>
       </c>
@@ -17883,7 +17911,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="267" spans="1:15">
+    <row r="267" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>282</v>
       </c>
@@ -17927,7 +17955,7 @@
         <v>1981</v>
       </c>
     </row>
-    <row r="268" spans="1:15">
+    <row r="268" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>283</v>
       </c>
@@ -17968,7 +17996,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="269" spans="1:15">
+    <row r="269" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>284</v>
       </c>
@@ -18006,7 +18034,7 @@
         <v>1757</v>
       </c>
     </row>
-    <row r="270" spans="1:15">
+    <row r="270" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>285</v>
       </c>
@@ -18047,7 +18075,7 @@
         <v>1943</v>
       </c>
     </row>
-    <row r="271" spans="1:15">
+    <row r="271" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>286</v>
       </c>
@@ -18088,7 +18116,7 @@
         <v>1982</v>
       </c>
     </row>
-    <row r="272" spans="1:15">
+    <row r="272" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>287</v>
       </c>
@@ -18129,7 +18157,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="273" spans="1:15">
+    <row r="273" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>288</v>
       </c>
@@ -18173,7 +18201,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="274" spans="1:15">
+    <row r="274" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>289</v>
       </c>
@@ -18214,7 +18242,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="275" spans="1:15">
+    <row r="275" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>290</v>
       </c>
@@ -18255,7 +18283,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="276" spans="1:15">
+    <row r="276" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>291</v>
       </c>
@@ -18299,7 +18327,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="277" spans="1:15">
+    <row r="277" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>292</v>
       </c>
@@ -18340,7 +18368,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="278" spans="1:15">
+    <row r="278" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>293</v>
       </c>
@@ -18378,7 +18406,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="279" spans="1:15">
+    <row r="279" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>294</v>
       </c>
@@ -18419,7 +18447,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="280" spans="1:15">
+    <row r="280" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>295</v>
       </c>
@@ -18460,7 +18488,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="281" spans="1:15">
+    <row r="281" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>296</v>
       </c>
@@ -18501,7 +18529,7 @@
         <v>1990</v>
       </c>
     </row>
-    <row r="282" spans="1:15">
+    <row r="282" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>297</v>
       </c>
@@ -18542,7 +18570,7 @@
         <v>1770</v>
       </c>
     </row>
-    <row r="283" spans="1:15">
+    <row r="283" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>298</v>
       </c>
@@ -18583,7 +18611,7 @@
         <v>1991</v>
       </c>
     </row>
-    <row r="284" spans="1:15">
+    <row r="284" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>299</v>
       </c>
@@ -18627,7 +18655,7 @@
         <v>1845</v>
       </c>
     </row>
-    <row r="285" spans="1:15">
+    <row r="285" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>300</v>
       </c>
@@ -18668,7 +18696,7 @@
         <v>1992</v>
       </c>
     </row>
-    <row r="286" spans="1:15">
+    <row r="286" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>301</v>
       </c>
@@ -18712,7 +18740,7 @@
         <v>1993</v>
       </c>
     </row>
-    <row r="287" spans="1:15">
+    <row r="287" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>302</v>
       </c>
@@ -18753,7 +18781,7 @@
         <v>1994</v>
       </c>
     </row>
-    <row r="288" spans="1:15">
+    <row r="288" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>303</v>
       </c>
@@ -18794,7 +18822,7 @@
         <v>1775</v>
       </c>
     </row>
-    <row r="289" spans="1:15">
+    <row r="289" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>304</v>
       </c>
@@ -18835,7 +18863,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="290" spans="1:15">
+    <row r="290" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>305</v>
       </c>
@@ -18876,7 +18904,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="291" spans="1:15">
+    <row r="291" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>306</v>
       </c>
@@ -18914,7 +18942,7 @@
         <v>1778</v>
       </c>
     </row>
-    <row r="292" spans="1:15">
+    <row r="292" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>307</v>
       </c>
@@ -18952,7 +18980,7 @@
         <v>1997</v>
       </c>
     </row>
-    <row r="293" spans="1:15">
+    <row r="293" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>308</v>
       </c>
@@ -18969,7 +18997,7 @@
         <v>1515</v>
       </c>
     </row>
-    <row r="294" spans="1:15">
+    <row r="294" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>309</v>
       </c>
@@ -18991,296 +19019,296 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F6" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F8" r:id="rId6"/>
-    <hyperlink ref="F9" r:id="rId7"/>
-    <hyperlink ref="F10" r:id="rId8"/>
-    <hyperlink ref="F11" r:id="rId9"/>
-    <hyperlink ref="F12" r:id="rId10"/>
-    <hyperlink ref="F13" r:id="rId11"/>
-    <hyperlink ref="F14" r:id="rId12"/>
-    <hyperlink ref="F15" r:id="rId13"/>
-    <hyperlink ref="F16" r:id="rId14"/>
-    <hyperlink ref="F17" r:id="rId15"/>
-    <hyperlink ref="F18" r:id="rId16"/>
-    <hyperlink ref="F19" r:id="rId17"/>
-    <hyperlink ref="F20" r:id="rId18"/>
-    <hyperlink ref="F21" r:id="rId19"/>
-    <hyperlink ref="F22" r:id="rId20"/>
-    <hyperlink ref="F23" r:id="rId21"/>
-    <hyperlink ref="F24" r:id="rId22"/>
-    <hyperlink ref="M24" r:id="rId23"/>
-    <hyperlink ref="M25" r:id="rId24"/>
-    <hyperlink ref="F27" r:id="rId25"/>
-    <hyperlink ref="F28" r:id="rId26"/>
-    <hyperlink ref="F29" r:id="rId27"/>
-    <hyperlink ref="F30" r:id="rId28"/>
-    <hyperlink ref="M30" r:id="rId29"/>
-    <hyperlink ref="F32" r:id="rId30"/>
-    <hyperlink ref="M32" r:id="rId31"/>
-    <hyperlink ref="F33" r:id="rId32"/>
-    <hyperlink ref="F34" r:id="rId33"/>
-    <hyperlink ref="F35" r:id="rId34"/>
-    <hyperlink ref="M35" r:id="rId35"/>
-    <hyperlink ref="F37" r:id="rId36"/>
-    <hyperlink ref="F38" r:id="rId37"/>
-    <hyperlink ref="F39" r:id="rId38"/>
-    <hyperlink ref="F40" r:id="rId39"/>
-    <hyperlink ref="M40" r:id="rId40"/>
-    <hyperlink ref="M41" r:id="rId41"/>
-    <hyperlink ref="M42" r:id="rId42"/>
-    <hyperlink ref="F44" r:id="rId43"/>
-    <hyperlink ref="F45" r:id="rId44"/>
-    <hyperlink ref="F46" r:id="rId45"/>
-    <hyperlink ref="F47" r:id="rId46"/>
-    <hyperlink ref="F48" r:id="rId47"/>
-    <hyperlink ref="F49" r:id="rId48"/>
-    <hyperlink ref="F50" r:id="rId49"/>
-    <hyperlink ref="F51" r:id="rId50"/>
-    <hyperlink ref="F52" r:id="rId51"/>
-    <hyperlink ref="M52" r:id="rId52"/>
-    <hyperlink ref="F54" r:id="rId53"/>
-    <hyperlink ref="F55" r:id="rId54"/>
-    <hyperlink ref="F56" r:id="rId55"/>
-    <hyperlink ref="M56" r:id="rId56"/>
-    <hyperlink ref="F58" r:id="rId57"/>
-    <hyperlink ref="F59" r:id="rId58"/>
-    <hyperlink ref="M59" r:id="rId59"/>
-    <hyperlink ref="F61" r:id="rId60"/>
-    <hyperlink ref="F62" r:id="rId61"/>
-    <hyperlink ref="F63" r:id="rId62"/>
-    <hyperlink ref="F64" r:id="rId63"/>
-    <hyperlink ref="F65" r:id="rId64"/>
-    <hyperlink ref="F66" r:id="rId65"/>
-    <hyperlink ref="M66" r:id="rId66"/>
-    <hyperlink ref="F68" r:id="rId67"/>
-    <hyperlink ref="F69" r:id="rId68"/>
-    <hyperlink ref="F70" r:id="rId69"/>
-    <hyperlink ref="M70" r:id="rId70"/>
-    <hyperlink ref="F72" r:id="rId71"/>
-    <hyperlink ref="F73" r:id="rId72"/>
-    <hyperlink ref="M73" r:id="rId73"/>
-    <hyperlink ref="F75" r:id="rId74"/>
-    <hyperlink ref="M75" r:id="rId75"/>
-    <hyperlink ref="M76" r:id="rId76"/>
-    <hyperlink ref="F78" r:id="rId77"/>
-    <hyperlink ref="M78" r:id="rId78"/>
-    <hyperlink ref="M79" r:id="rId79"/>
-    <hyperlink ref="F82" r:id="rId80"/>
-    <hyperlink ref="F83" r:id="rId81"/>
-    <hyperlink ref="F84" r:id="rId82"/>
-    <hyperlink ref="M84" r:id="rId83"/>
-    <hyperlink ref="M86" r:id="rId84"/>
-    <hyperlink ref="F88" r:id="rId85"/>
-    <hyperlink ref="F89" r:id="rId86"/>
-    <hyperlink ref="M89" r:id="rId87"/>
-    <hyperlink ref="M90" r:id="rId88"/>
-    <hyperlink ref="F91" r:id="rId89"/>
-    <hyperlink ref="M91" r:id="rId90"/>
-    <hyperlink ref="F93" r:id="rId91"/>
-    <hyperlink ref="M93" r:id="rId92"/>
-    <hyperlink ref="F95" r:id="rId93"/>
-    <hyperlink ref="M95" r:id="rId94"/>
-    <hyperlink ref="M96" r:id="rId95"/>
-    <hyperlink ref="M97" r:id="rId96"/>
-    <hyperlink ref="M98" r:id="rId97"/>
-    <hyperlink ref="F100" r:id="rId98"/>
-    <hyperlink ref="M100" r:id="rId99"/>
-    <hyperlink ref="F103" r:id="rId100"/>
-    <hyperlink ref="F104" r:id="rId101"/>
-    <hyperlink ref="F105" r:id="rId102"/>
-    <hyperlink ref="M105" r:id="rId103"/>
-    <hyperlink ref="F107" r:id="rId104"/>
-    <hyperlink ref="F108" r:id="rId105"/>
-    <hyperlink ref="F109" r:id="rId106"/>
-    <hyperlink ref="F110" r:id="rId107"/>
-    <hyperlink ref="F111" r:id="rId108"/>
-    <hyperlink ref="M111" r:id="rId109"/>
-    <hyperlink ref="F113" r:id="rId110"/>
-    <hyperlink ref="F114" r:id="rId111"/>
-    <hyperlink ref="F115" r:id="rId112"/>
-    <hyperlink ref="F116" r:id="rId113"/>
-    <hyperlink ref="F117" r:id="rId114"/>
-    <hyperlink ref="F119" r:id="rId115"/>
-    <hyperlink ref="F120" r:id="rId116"/>
-    <hyperlink ref="F121" r:id="rId117"/>
-    <hyperlink ref="F122" r:id="rId118"/>
-    <hyperlink ref="F123" r:id="rId119"/>
-    <hyperlink ref="F124" r:id="rId120"/>
-    <hyperlink ref="F125" r:id="rId121"/>
-    <hyperlink ref="F126" r:id="rId122"/>
-    <hyperlink ref="F127" r:id="rId123"/>
-    <hyperlink ref="M127" r:id="rId124"/>
-    <hyperlink ref="F129" r:id="rId125"/>
-    <hyperlink ref="F130" r:id="rId126"/>
-    <hyperlink ref="F131" r:id="rId127"/>
-    <hyperlink ref="F132" r:id="rId128"/>
-    <hyperlink ref="F133" r:id="rId129"/>
-    <hyperlink ref="M133" r:id="rId130"/>
-    <hyperlink ref="F136" r:id="rId131"/>
-    <hyperlink ref="M136" r:id="rId132"/>
-    <hyperlink ref="F138" r:id="rId133"/>
-    <hyperlink ref="F139" r:id="rId134"/>
-    <hyperlink ref="M139" r:id="rId135"/>
-    <hyperlink ref="F141" r:id="rId136"/>
-    <hyperlink ref="M141" r:id="rId137"/>
-    <hyperlink ref="F142" r:id="rId138"/>
-    <hyperlink ref="F143" r:id="rId139"/>
-    <hyperlink ref="M143" r:id="rId140"/>
-    <hyperlink ref="F145" r:id="rId141"/>
-    <hyperlink ref="F146" r:id="rId142"/>
-    <hyperlink ref="F147" r:id="rId143"/>
-    <hyperlink ref="F148" r:id="rId144"/>
-    <hyperlink ref="F150" r:id="rId145"/>
-    <hyperlink ref="F151" r:id="rId146"/>
-    <hyperlink ref="M151" r:id="rId147"/>
-    <hyperlink ref="F153" r:id="rId148"/>
-    <hyperlink ref="F154" r:id="rId149"/>
-    <hyperlink ref="F155" r:id="rId150"/>
-    <hyperlink ref="F156" r:id="rId151"/>
-    <hyperlink ref="M156" r:id="rId152"/>
-    <hyperlink ref="M157" r:id="rId153"/>
-    <hyperlink ref="M158" r:id="rId154"/>
-    <hyperlink ref="M159" r:id="rId155"/>
-    <hyperlink ref="F161" r:id="rId156"/>
-    <hyperlink ref="F162" r:id="rId157"/>
-    <hyperlink ref="M162" r:id="rId158"/>
-    <hyperlink ref="F164" r:id="rId159"/>
-    <hyperlink ref="F165" r:id="rId160"/>
-    <hyperlink ref="F166" r:id="rId161"/>
-    <hyperlink ref="M166" r:id="rId162"/>
-    <hyperlink ref="M167" r:id="rId163"/>
-    <hyperlink ref="F169" r:id="rId164"/>
-    <hyperlink ref="F170" r:id="rId165"/>
-    <hyperlink ref="F171" r:id="rId166"/>
-    <hyperlink ref="F172" r:id="rId167"/>
-    <hyperlink ref="F174" r:id="rId168"/>
-    <hyperlink ref="M174" r:id="rId169"/>
-    <hyperlink ref="F176" r:id="rId170"/>
-    <hyperlink ref="F177" r:id="rId171"/>
-    <hyperlink ref="F178" r:id="rId172"/>
-    <hyperlink ref="F179" r:id="rId173"/>
-    <hyperlink ref="F180" r:id="rId174"/>
-    <hyperlink ref="F181" r:id="rId175"/>
-    <hyperlink ref="F182" r:id="rId176"/>
-    <hyperlink ref="F183" r:id="rId177"/>
-    <hyperlink ref="F184" r:id="rId178"/>
-    <hyperlink ref="F185" r:id="rId179"/>
-    <hyperlink ref="F186" r:id="rId180"/>
-    <hyperlink ref="F187" r:id="rId181"/>
-    <hyperlink ref="F188" r:id="rId182"/>
-    <hyperlink ref="F189" r:id="rId183"/>
-    <hyperlink ref="M189" r:id="rId184"/>
-    <hyperlink ref="F191" r:id="rId185"/>
-    <hyperlink ref="F192" r:id="rId186"/>
-    <hyperlink ref="M192" r:id="rId187"/>
-    <hyperlink ref="F194" r:id="rId188"/>
-    <hyperlink ref="F195" r:id="rId189"/>
-    <hyperlink ref="F196" r:id="rId190"/>
-    <hyperlink ref="M196" r:id="rId191"/>
-    <hyperlink ref="F198" r:id="rId192"/>
-    <hyperlink ref="F199" r:id="rId193"/>
-    <hyperlink ref="F200" r:id="rId194"/>
-    <hyperlink ref="M200" r:id="rId195"/>
-    <hyperlink ref="M201" r:id="rId196"/>
-    <hyperlink ref="F203" r:id="rId197"/>
-    <hyperlink ref="M203" r:id="rId198"/>
-    <hyperlink ref="F205" r:id="rId199"/>
-    <hyperlink ref="F206" r:id="rId200"/>
-    <hyperlink ref="M206" r:id="rId201"/>
-    <hyperlink ref="F208" r:id="rId202"/>
-    <hyperlink ref="F209" r:id="rId203"/>
-    <hyperlink ref="M209" r:id="rId204"/>
-    <hyperlink ref="M210" r:id="rId205"/>
-    <hyperlink ref="M211" r:id="rId206"/>
-    <hyperlink ref="F212" r:id="rId207"/>
-    <hyperlink ref="F213" r:id="rId208"/>
-    <hyperlink ref="F214" r:id="rId209"/>
-    <hyperlink ref="F215" r:id="rId210"/>
-    <hyperlink ref="F216" r:id="rId211"/>
-    <hyperlink ref="M216" r:id="rId212"/>
-    <hyperlink ref="F218" r:id="rId213"/>
-    <hyperlink ref="M218" r:id="rId214"/>
-    <hyperlink ref="F220" r:id="rId215"/>
-    <hyperlink ref="M220" r:id="rId216"/>
-    <hyperlink ref="F222" r:id="rId217"/>
-    <hyperlink ref="M222" r:id="rId218" location="zoom=50&#10;https://www.accenture.com/gb-en/services/data-ai/responsible-ai?form=MG0AV3"/>
-    <hyperlink ref="F224" r:id="rId219"/>
-    <hyperlink ref="F225" r:id="rId220"/>
-    <hyperlink ref="M225" r:id="rId221"/>
-    <hyperlink ref="F227" r:id="rId222"/>
-    <hyperlink ref="F228" r:id="rId223"/>
-    <hyperlink ref="M228" r:id="rId224"/>
-    <hyperlink ref="M229" r:id="rId225"/>
-    <hyperlink ref="M230" r:id="rId226"/>
-    <hyperlink ref="M231" r:id="rId227"/>
-    <hyperlink ref="M232" r:id="rId228"/>
-    <hyperlink ref="M233" r:id="rId229"/>
-    <hyperlink ref="M234" r:id="rId230"/>
-    <hyperlink ref="M235" r:id="rId231"/>
-    <hyperlink ref="M236" r:id="rId232"/>
-    <hyperlink ref="M237" r:id="rId233"/>
-    <hyperlink ref="M238" r:id="rId234"/>
-    <hyperlink ref="F240" r:id="rId235"/>
-    <hyperlink ref="M240" r:id="rId236"/>
-    <hyperlink ref="M241" r:id="rId237"/>
-    <hyperlink ref="F242" r:id="rId238"/>
-    <hyperlink ref="M242" r:id="rId239"/>
-    <hyperlink ref="M243" r:id="rId240"/>
-    <hyperlink ref="F245" r:id="rId241"/>
-    <hyperlink ref="F246" r:id="rId242"/>
-    <hyperlink ref="M246" r:id="rId243"/>
-    <hyperlink ref="F248" r:id="rId244"/>
-    <hyperlink ref="M249" r:id="rId245"/>
-    <hyperlink ref="M250" r:id="rId246"/>
-    <hyperlink ref="F252" r:id="rId247"/>
-    <hyperlink ref="F253" r:id="rId248"/>
-    <hyperlink ref="F254" r:id="rId249"/>
-    <hyperlink ref="F255" r:id="rId250"/>
-    <hyperlink ref="F256" r:id="rId251"/>
-    <hyperlink ref="F257" r:id="rId252"/>
-    <hyperlink ref="M257" r:id="rId253"/>
-    <hyperlink ref="M258" r:id="rId254"/>
-    <hyperlink ref="F260" r:id="rId255"/>
-    <hyperlink ref="F261" r:id="rId256"/>
-    <hyperlink ref="F263" r:id="rId257"/>
-    <hyperlink ref="F264" r:id="rId258"/>
-    <hyperlink ref="M264" r:id="rId259"/>
-    <hyperlink ref="F266" r:id="rId260"/>
-    <hyperlink ref="F267" r:id="rId261"/>
-    <hyperlink ref="F268" r:id="rId262"/>
-    <hyperlink ref="M268" r:id="rId263"/>
-    <hyperlink ref="M269" r:id="rId264"/>
-    <hyperlink ref="M270" r:id="rId265"/>
-    <hyperlink ref="M271" r:id="rId266"/>
-    <hyperlink ref="F273" r:id="rId267"/>
-    <hyperlink ref="F274" r:id="rId268"/>
-    <hyperlink ref="M274" r:id="rId269"/>
-    <hyperlink ref="F276" r:id="rId270"/>
-    <hyperlink ref="M276" r:id="rId271"/>
-    <hyperlink ref="M277" r:id="rId272"/>
-    <hyperlink ref="M278" r:id="rId273"/>
-    <hyperlink ref="M279" r:id="rId274"/>
-    <hyperlink ref="M280" r:id="rId275"/>
-    <hyperlink ref="F282" r:id="rId276"/>
-    <hyperlink ref="M282" r:id="rId277"/>
-    <hyperlink ref="F284" r:id="rId278"/>
-    <hyperlink ref="M284" r:id="rId279"/>
-    <hyperlink ref="F286" r:id="rId280"/>
-    <hyperlink ref="M286" r:id="rId281"/>
-    <hyperlink ref="F288" r:id="rId282"/>
-    <hyperlink ref="M288" r:id="rId283"/>
-    <hyperlink ref="M289" r:id="rId284"/>
-    <hyperlink ref="M290" r:id="rId285"/>
-    <hyperlink ref="M291" r:id="rId286"/>
-    <hyperlink ref="M292" r:id="rId287"/>
-    <hyperlink ref="M293" r:id="rId288"/>
-    <hyperlink ref="F294" r:id="rId289"/>
-    <hyperlink ref="M294" r:id="rId290"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F21" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F22" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="M24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="M25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F27" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F28" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F29" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="M30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F32" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="M32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="M35" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="M40" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="M41" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="M42" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="M52" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="M56" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="M59" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="M66" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="M70" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="M73" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="M75" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="M76" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="F78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="M78" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="M79" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="F82" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="F83" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="F84" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="M84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="M86" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="F88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="F89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="M89" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="M90" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="F91" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="M91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="F93" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="M93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="F95" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="M95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="M96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="M97" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="M98" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="F100" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="M100" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="F103" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="F104" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="F105" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="M105" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="F107" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="F108" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="F109" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="F110" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="F111" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="M111" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="F113" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="F114" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="F115" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="F116" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="F117" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="F119" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="F120" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="F121" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="F122" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="F123" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="F124" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="F125" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="F126" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="F127" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="M127" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="F129" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="F130" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="F131" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="F132" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="F133" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="M133" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="F136" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="M136" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="F138" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="F139" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="M139" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="F141" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="M141" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="F142" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="F143" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="M143" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="F145" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="F146" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="F147" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="F148" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="F150" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="F151" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="M151" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="F153" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="F154" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="F155" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="F156" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="M156" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="M157" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="M158" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="M159" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="F161" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="F162" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="M162" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="F164" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="F165" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="F166" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="M166" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="M167" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="F169" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="F170" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="F171" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="F172" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="F174" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="M174" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="F176" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="F177" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="F178" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="F179" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="F180" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="F181" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="F182" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="F183" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="F184" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="F185" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="F186" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="F187" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="F188" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="F189" r:id="rId183" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="M189" r:id="rId184" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="F191" r:id="rId185" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="F192" r:id="rId186" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="M192" r:id="rId187" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="F194" r:id="rId188" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="F195" r:id="rId189" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="F196" r:id="rId190" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="M196" r:id="rId191" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="F198" r:id="rId192" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="F199" r:id="rId193" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="F200" r:id="rId194" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="M200" r:id="rId195" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="M201" r:id="rId196" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="F203" r:id="rId197" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="M203" r:id="rId198" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="F205" r:id="rId199" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="F206" r:id="rId200" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="M206" r:id="rId201" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="F208" r:id="rId202" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="F209" r:id="rId203" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="M209" r:id="rId204" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="M210" r:id="rId205" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="M211" r:id="rId206" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="F212" r:id="rId207" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="F213" r:id="rId208" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="F214" r:id="rId209" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="F215" r:id="rId210" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="F216" r:id="rId211" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="M216" r:id="rId212" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="F218" r:id="rId213" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="M218" r:id="rId214" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="F220" r:id="rId215" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="M220" r:id="rId216" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="F222" r:id="rId217" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="M222" r:id="rId218" location="zoom=50_x000a_https://www.accenture.com/gb-en/services/data-ai/responsible-ai?form=MG0AV3" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="F224" r:id="rId219" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="F225" r:id="rId220" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="M225" r:id="rId221" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="F227" r:id="rId222" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="F228" r:id="rId223" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="M228" r:id="rId224" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="M229" r:id="rId225" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="M230" r:id="rId226" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="M231" r:id="rId227" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="M232" r:id="rId228" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="M233" r:id="rId229" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="M234" r:id="rId230" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="M235" r:id="rId231" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="M236" r:id="rId232" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="M237" r:id="rId233" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
+    <hyperlink ref="M238" r:id="rId234" xr:uid="{00000000-0004-0000-0000-0000E9000000}"/>
+    <hyperlink ref="F240" r:id="rId235" xr:uid="{00000000-0004-0000-0000-0000EA000000}"/>
+    <hyperlink ref="M240" r:id="rId236" xr:uid="{00000000-0004-0000-0000-0000EB000000}"/>
+    <hyperlink ref="M241" r:id="rId237" xr:uid="{00000000-0004-0000-0000-0000EC000000}"/>
+    <hyperlink ref="F242" r:id="rId238" xr:uid="{00000000-0004-0000-0000-0000ED000000}"/>
+    <hyperlink ref="M242" r:id="rId239" xr:uid="{00000000-0004-0000-0000-0000EE000000}"/>
+    <hyperlink ref="M243" r:id="rId240" xr:uid="{00000000-0004-0000-0000-0000EF000000}"/>
+    <hyperlink ref="F245" r:id="rId241" xr:uid="{00000000-0004-0000-0000-0000F0000000}"/>
+    <hyperlink ref="F246" r:id="rId242" xr:uid="{00000000-0004-0000-0000-0000F1000000}"/>
+    <hyperlink ref="M246" r:id="rId243" xr:uid="{00000000-0004-0000-0000-0000F2000000}"/>
+    <hyperlink ref="F248" r:id="rId244" xr:uid="{00000000-0004-0000-0000-0000F3000000}"/>
+    <hyperlink ref="M249" r:id="rId245" xr:uid="{00000000-0004-0000-0000-0000F4000000}"/>
+    <hyperlink ref="M250" r:id="rId246" xr:uid="{00000000-0004-0000-0000-0000F5000000}"/>
+    <hyperlink ref="F252" r:id="rId247" xr:uid="{00000000-0004-0000-0000-0000F6000000}"/>
+    <hyperlink ref="F253" r:id="rId248" xr:uid="{00000000-0004-0000-0000-0000F7000000}"/>
+    <hyperlink ref="F254" r:id="rId249" xr:uid="{00000000-0004-0000-0000-0000F8000000}"/>
+    <hyperlink ref="F255" r:id="rId250" xr:uid="{00000000-0004-0000-0000-0000F9000000}"/>
+    <hyperlink ref="F256" r:id="rId251" xr:uid="{00000000-0004-0000-0000-0000FA000000}"/>
+    <hyperlink ref="F257" r:id="rId252" xr:uid="{00000000-0004-0000-0000-0000FB000000}"/>
+    <hyperlink ref="M257" r:id="rId253" xr:uid="{00000000-0004-0000-0000-0000FC000000}"/>
+    <hyperlink ref="M258" r:id="rId254" xr:uid="{00000000-0004-0000-0000-0000FD000000}"/>
+    <hyperlink ref="F260" r:id="rId255" xr:uid="{00000000-0004-0000-0000-0000FE000000}"/>
+    <hyperlink ref="F261" r:id="rId256" xr:uid="{00000000-0004-0000-0000-0000FF000000}"/>
+    <hyperlink ref="F263" r:id="rId257" xr:uid="{00000000-0004-0000-0000-000000010000}"/>
+    <hyperlink ref="F264" r:id="rId258" xr:uid="{00000000-0004-0000-0000-000001010000}"/>
+    <hyperlink ref="M264" r:id="rId259" xr:uid="{00000000-0004-0000-0000-000002010000}"/>
+    <hyperlink ref="F266" r:id="rId260" xr:uid="{00000000-0004-0000-0000-000003010000}"/>
+    <hyperlink ref="F267" r:id="rId261" xr:uid="{00000000-0004-0000-0000-000004010000}"/>
+    <hyperlink ref="F268" r:id="rId262" xr:uid="{00000000-0004-0000-0000-000005010000}"/>
+    <hyperlink ref="M268" r:id="rId263" xr:uid="{00000000-0004-0000-0000-000006010000}"/>
+    <hyperlink ref="M269" r:id="rId264" xr:uid="{00000000-0004-0000-0000-000007010000}"/>
+    <hyperlink ref="M270" r:id="rId265" xr:uid="{00000000-0004-0000-0000-000008010000}"/>
+    <hyperlink ref="M271" r:id="rId266" xr:uid="{00000000-0004-0000-0000-000009010000}"/>
+    <hyperlink ref="F273" r:id="rId267" xr:uid="{00000000-0004-0000-0000-00000A010000}"/>
+    <hyperlink ref="F274" r:id="rId268" xr:uid="{00000000-0004-0000-0000-00000B010000}"/>
+    <hyperlink ref="M274" r:id="rId269" xr:uid="{00000000-0004-0000-0000-00000C010000}"/>
+    <hyperlink ref="F276" r:id="rId270" xr:uid="{00000000-0004-0000-0000-00000D010000}"/>
+    <hyperlink ref="M276" r:id="rId271" xr:uid="{00000000-0004-0000-0000-00000E010000}"/>
+    <hyperlink ref="M277" r:id="rId272" xr:uid="{00000000-0004-0000-0000-00000F010000}"/>
+    <hyperlink ref="M278" r:id="rId273" xr:uid="{00000000-0004-0000-0000-000010010000}"/>
+    <hyperlink ref="M279" r:id="rId274" xr:uid="{00000000-0004-0000-0000-000011010000}"/>
+    <hyperlink ref="M280" r:id="rId275" xr:uid="{00000000-0004-0000-0000-000012010000}"/>
+    <hyperlink ref="F282" r:id="rId276" xr:uid="{00000000-0004-0000-0000-000013010000}"/>
+    <hyperlink ref="M282" r:id="rId277" xr:uid="{00000000-0004-0000-0000-000014010000}"/>
+    <hyperlink ref="F284" r:id="rId278" xr:uid="{00000000-0004-0000-0000-000015010000}"/>
+    <hyperlink ref="M284" r:id="rId279" xr:uid="{00000000-0004-0000-0000-000016010000}"/>
+    <hyperlink ref="F286" r:id="rId280" xr:uid="{00000000-0004-0000-0000-000017010000}"/>
+    <hyperlink ref="M286" r:id="rId281" xr:uid="{00000000-0004-0000-0000-000018010000}"/>
+    <hyperlink ref="F288" r:id="rId282" xr:uid="{00000000-0004-0000-0000-000019010000}"/>
+    <hyperlink ref="M288" r:id="rId283" xr:uid="{00000000-0004-0000-0000-00001A010000}"/>
+    <hyperlink ref="M289" r:id="rId284" xr:uid="{00000000-0004-0000-0000-00001B010000}"/>
+    <hyperlink ref="M290" r:id="rId285" xr:uid="{00000000-0004-0000-0000-00001C010000}"/>
+    <hyperlink ref="M291" r:id="rId286" xr:uid="{00000000-0004-0000-0000-00001D010000}"/>
+    <hyperlink ref="M292" r:id="rId287" xr:uid="{00000000-0004-0000-0000-00001E010000}"/>
+    <hyperlink ref="M293" r:id="rId288" xr:uid="{00000000-0004-0000-0000-00001F010000}"/>
+    <hyperlink ref="F294" r:id="rId289" xr:uid="{00000000-0004-0000-0000-000020010000}"/>
+    <hyperlink ref="M294" r:id="rId290" xr:uid="{00000000-0004-0000-0000-000021010000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>